<commit_message>
crit path changed, outputs added
</commit_message>
<xml_diff>
--- a/Assignment4/outputs/critical_path_delays.xlsx
+++ b/Assignment4/outputs/critical_path_delays.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hemanth Ram\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Acads\Sem7\EE5311_Digital_IC_Design\EE5311-Digital-IC-Design\Assignment4\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87CA45A1-27AD-423D-88F9-4CE11A2B5983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2DCDD-5297-45FC-8114-7C44817C0F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{75A2B2A3-B3E2-432F-A7DC-EC91B0A9FA4A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75A2B2A3-B3E2-432F-A7DC-EC91B0A9FA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="20">
   <si>
     <t>wc=1</t>
   </si>
@@ -71,13 +71,34 @@
   </si>
   <si>
     <t>TO</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +106,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,14 +141,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -124,6 +202,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{883F346D-0899-4049-853C-B78402E0813D}" name="Table2" displayName="Table2" ref="A1:G29" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G29" xr:uid="{883F346D-0899-4049-853C-B78402E0813D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E70F29A0-85CB-4ED2-BFFE-8BEDD6F88C88}" name="Column1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A71068C3-BA12-47EC-A9B0-61478BADD54C}" name="Column2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{324AC005-7299-402A-96B4-0EA2CCA01A2C}" name="Column3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{6A7A012C-F4EE-47C8-9E3A-A999F3F109B2}" name="Column4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C687825B-9597-47C1-A4A8-6F772B5F0BAE}" name="Column6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1534F2EA-4AB2-4A6C-B893-507AE254E878}" name="Column7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{BD87819F-BAFA-4382-B09E-CA340C4EE2F4}" name="Column8" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,650 +517,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FD03E4-BA0E-4DE5-947F-78562A2D1CD3}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.21875" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="E3" s="4">
         <v>5.5445600000000003E-10</v>
       </c>
-      <c r="G2" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F3" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G3" s="4">
         <v>1.6044600000000001E-9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E4" s="4">
         <v>4.7282699999999998E-10</v>
       </c>
-      <c r="G3" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="F4" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G4" s="4">
         <v>1.52283E-9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="E5" s="4">
         <v>4.6381699999999998E-10</v>
       </c>
-      <c r="G4" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="F5" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G5" s="4">
         <v>1.5138200000000001E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="E6" s="4">
         <v>5.9765300000000002E-10</v>
       </c>
-      <c r="G5" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="F6" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G6" s="4">
         <v>1.64765E-9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="E7" s="4">
         <v>4.6537099999999997E-10</v>
       </c>
-      <c r="G6" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="F7" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G7" s="4">
         <v>1.5153699999999999E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="E8" s="4">
         <v>4.3243500000000002E-10</v>
       </c>
-      <c r="G7" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="F8" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G8" s="4">
         <v>1.48243E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="E9" s="4">
         <v>6.8190899999999997E-10</v>
       </c>
-      <c r="G8" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F9" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G9" s="4">
         <v>1.7319100000000001E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="1">
+      <c r="E10" s="4">
         <v>5.0318799999999998E-10</v>
       </c>
-      <c r="G9" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="F10" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G10" s="4">
         <v>1.5531900000000001E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="E11" s="4">
         <v>4.52091E-10</v>
       </c>
-      <c r="G10" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="F11" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G11" s="4">
         <v>1.5020899999999999E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="1">
+      <c r="E12" s="4">
         <v>5.50981E-10</v>
       </c>
-      <c r="G11" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="F12" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G12" s="4">
         <v>1.60098E-9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="1">
+      <c r="E13" s="4">
         <v>4.6684000000000001E-10</v>
       </c>
-      <c r="G12" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="F13" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G13" s="4">
         <v>1.5168399999999999E-9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="1">
+      <c r="E14" s="4">
         <v>4.5627899999999999E-10</v>
       </c>
-      <c r="G13" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F14" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G14" s="4">
         <v>1.5062800000000001E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="1">
+      <c r="E15" s="4">
         <v>5.9162900000000005E-10</v>
       </c>
-      <c r="G14" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="F15" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G15" s="4">
         <v>1.64163E-9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="1">
+      <c r="E16" s="4">
         <v>4.57087E-10</v>
       </c>
-      <c r="G15" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F16" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G16" s="4">
         <v>1.50709E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="1">
+      <c r="E17" s="4">
         <v>4.2276399999999998E-10</v>
       </c>
-      <c r="G16" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="F17" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G17" s="4">
         <v>1.47276E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="1">
+      <c r="E18" s="4">
         <v>6.7402599999999996E-10</v>
       </c>
-      <c r="G17" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F18" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G18" s="4">
         <v>1.7240300000000001E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="1">
+      <c r="E19" s="4">
         <v>4.9326799999999998E-10</v>
       </c>
-      <c r="G18" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F19" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G19" s="4">
         <v>1.54327E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="1">
+      <c r="E20" s="4">
         <v>4.4090700000000001E-10</v>
       </c>
-      <c r="G19" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="F20" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G20" s="4">
         <v>1.49091E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="1">
+      <c r="E21" s="4">
         <v>5.5419699999999998E-10</v>
       </c>
-      <c r="G20" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="F21" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G21" s="4">
         <v>1.6041999999999999E-9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="1">
+      <c r="E22" s="4">
         <v>4.6697400000000003E-10</v>
       </c>
-      <c r="G21" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="F22" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G22" s="4">
         <v>1.51697E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="1">
+      <c r="E23" s="4">
         <v>4.54864E-10</v>
       </c>
-      <c r="G22" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="F23" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G23" s="4">
         <v>1.5048599999999999E-9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="1">
+      <c r="E24" s="4">
         <v>5.9216900000000003E-10</v>
       </c>
-      <c r="G23" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="F24" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G24" s="4">
         <v>1.6421699999999999E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="1">
+      <c r="E25" s="4">
         <v>4.5466899999999998E-10</v>
       </c>
-      <c r="G24" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="F25" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G25" s="4">
         <v>1.5046699999999999E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="1">
+      <c r="E26" s="6">
         <v>4.1893199999999999E-10</v>
       </c>
-      <c r="G25" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F26" s="6">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G26" s="6">
         <v>1.46893E-9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="1">
+      <c r="E27" s="4">
         <v>6.7306800000000002E-10</v>
       </c>
-      <c r="G26" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="F27" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G27" s="4">
         <v>1.7230699999999999E-9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="1">
+      <c r="E28" s="4">
         <v>4.8947900000000004E-10</v>
       </c>
-      <c r="G27" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F28" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G28" s="4">
         <v>1.5394799999999999E-9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="1">
+      <c r="E29" s="4">
         <v>4.3581000000000002E-10</v>
       </c>
-      <c r="G28" s="1">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="F29" s="4">
+        <v>1.0500000000000001E-9</v>
+      </c>
+      <c r="G29" s="4">
         <v>1.4858100000000001E-9</v>
       </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected crit path, added report
</commit_message>
<xml_diff>
--- a/Assignment4/outputs/critical_path_delays.xlsx
+++ b/Assignment4/outputs/critical_path_delays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Acads\Sem7\EE5311_Digital_IC_Design\EE5311-Digital-IC-Design\Assignment4\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2DCDD-5297-45FC-8114-7C44817C0F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E126D05F-5CE6-4AE4-8FF5-A0BBDE9CDEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75A2B2A3-B3E2-432F-A7DC-EC91B0A9FA4A}"/>
   </bookViews>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FD03E4-BA0E-4DE5-947F-78562A2D1CD3}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
     <col min="6" max="7" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -556,7 +556,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -573,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -587,16 +587,19 @@
         <v>2</v>
       </c>
       <c r="E3" s="4">
-        <v>5.5445600000000003E-10</v>
+        <v>5.8686099999999999E-10</v>
       </c>
       <c r="F3" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G3" s="4">
-        <v>1.6044600000000001E-9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.6368600000000001E-9</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -610,16 +613,19 @@
         <v>2</v>
       </c>
       <c r="E4" s="4">
-        <v>4.7282699999999998E-10</v>
+        <v>4.94151E-10</v>
       </c>
       <c r="F4" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G4" s="4">
-        <v>1.52283E-9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5441500000000001E-9</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -633,16 +639,19 @@
         <v>2</v>
       </c>
       <c r="E5" s="4">
-        <v>4.6381699999999998E-10</v>
+        <v>4.8245599999999997E-10</v>
       </c>
       <c r="F5" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G5" s="4">
-        <v>1.5138200000000001E-9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5324599999999999E-9</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -656,16 +665,19 @@
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <v>5.9765300000000002E-10</v>
+        <v>6.0946500000000002E-10</v>
       </c>
       <c r="F6" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G6" s="4">
-        <v>1.64765E-9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.6594700000000001E-9</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -679,16 +691,19 @@
         <v>2</v>
       </c>
       <c r="E7" s="4">
-        <v>4.6537099999999997E-10</v>
+        <v>4.6347E-10</v>
       </c>
       <c r="F7" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G7" s="4">
-        <v>1.5153699999999999E-9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5134699999999999E-9</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -702,16 +717,19 @@
         <v>2</v>
       </c>
       <c r="E8" s="4">
-        <v>4.3243500000000002E-10</v>
+        <v>4.2534899999999998E-10</v>
       </c>
       <c r="F8" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G8" s="4">
-        <v>1.48243E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.4753500000000001E-9</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -725,16 +743,19 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <v>6.8190899999999997E-10</v>
+        <v>6.8123599999999998E-10</v>
       </c>
       <c r="F9" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G9" s="4">
-        <v>1.7319100000000001E-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.7312399999999999E-9</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -748,16 +769,19 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <v>5.0318799999999998E-10</v>
+        <v>4.8687999999999998E-10</v>
       </c>
       <c r="F10" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G10" s="4">
-        <v>1.5531900000000001E-9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.53688E-9</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -771,16 +795,19 @@
         <v>2</v>
       </c>
       <c r="E11" s="4">
-        <v>4.52091E-10</v>
+        <v>4.2908400000000001E-10</v>
       </c>
       <c r="F11" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G11" s="4">
-        <v>1.5020899999999999E-9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.47908E-9</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -794,16 +821,19 @@
         <v>7</v>
       </c>
       <c r="E12" s="4">
-        <v>5.50981E-10</v>
+        <v>5.8271199999999996E-10</v>
       </c>
       <c r="F12" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G12" s="4">
-        <v>1.60098E-9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.63271E-9</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -817,16 +847,19 @@
         <v>7</v>
       </c>
       <c r="E13" s="4">
-        <v>4.6684000000000001E-10</v>
+        <v>4.8757699999999996E-10</v>
       </c>
       <c r="F13" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G13" s="4">
-        <v>1.5168399999999999E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.53758E-9</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -840,16 +873,19 @@
         <v>7</v>
       </c>
       <c r="E14" s="4">
-        <v>4.5627899999999999E-10</v>
+        <v>4.7430500000000005E-10</v>
       </c>
       <c r="F14" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G14" s="4">
-        <v>1.5062800000000001E-9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5243E-9</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -863,16 +899,19 @@
         <v>7</v>
       </c>
       <c r="E15" s="4">
-        <v>5.9162900000000005E-10</v>
+        <v>6.0249700000000001E-10</v>
       </c>
       <c r="F15" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G15" s="4">
-        <v>1.64163E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.6525E-9</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -886,16 +925,19 @@
         <v>7</v>
       </c>
       <c r="E16" s="4">
-        <v>4.57087E-10</v>
+        <v>4.54382E-10</v>
       </c>
       <c r="F16" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G16" s="4">
-        <v>1.50709E-9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5043799999999999E-9</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -909,16 +951,19 @@
         <v>7</v>
       </c>
       <c r="E17" s="4">
-        <v>4.2276399999999998E-10</v>
+        <v>4.1492499999999999E-10</v>
       </c>
       <c r="F17" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G17" s="4">
-        <v>1.47276E-9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.46493E-9</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -932,16 +977,19 @@
         <v>7</v>
       </c>
       <c r="E18" s="4">
-        <v>6.7402599999999996E-10</v>
+        <v>6.7233699999999995E-10</v>
       </c>
       <c r="F18" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G18" s="4">
-        <v>1.7240300000000001E-9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.7223400000000001E-9</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -955,16 +1003,19 @@
         <v>7</v>
       </c>
       <c r="E19" s="4">
-        <v>4.9326799999999998E-10</v>
+        <v>4.7595E-10</v>
       </c>
       <c r="F19" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G19" s="4">
-        <v>1.54327E-9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5259500000000001E-9</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -978,16 +1029,19 @@
         <v>7</v>
       </c>
       <c r="E20" s="4">
-        <v>4.4090700000000001E-10</v>
+        <v>4.1686200000000001E-10</v>
       </c>
       <c r="F20" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G20" s="4">
-        <v>1.49091E-9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.46686E-9</v>
+      </c>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1001,16 +1055,19 @@
         <v>8</v>
       </c>
       <c r="E21" s="4">
-        <v>5.5419699999999998E-10</v>
+        <v>5.8547299999999997E-10</v>
       </c>
       <c r="F21" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G21" s="4">
-        <v>1.6041999999999999E-9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.6354699999999999E-9</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1024,16 +1081,19 @@
         <v>8</v>
       </c>
       <c r="E22" s="4">
-        <v>4.6697400000000003E-10</v>
+        <v>4.8737599999999999E-10</v>
       </c>
       <c r="F22" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G22" s="4">
-        <v>1.51697E-9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5373799999999999E-9</v>
+      </c>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1047,16 +1107,19 @@
         <v>8</v>
       </c>
       <c r="E23" s="4">
-        <v>4.54864E-10</v>
+        <v>4.7260500000000004E-10</v>
       </c>
       <c r="F23" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G23" s="4">
-        <v>1.5048599999999999E-9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5226000000000001E-9</v>
+      </c>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1070,16 +1133,19 @@
         <v>8</v>
       </c>
       <c r="E24" s="4">
-        <v>5.9216900000000003E-10</v>
+        <v>6.0237600000000001E-10</v>
       </c>
       <c r="F24" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G24" s="4">
-        <v>1.6421699999999999E-9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.65238E-9</v>
+      </c>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1093,16 +1159,19 @@
         <v>8</v>
       </c>
       <c r="E25" s="4">
-        <v>4.5466899999999998E-10</v>
+        <v>4.5149199999999997E-10</v>
       </c>
       <c r="F25" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G25" s="4">
-        <v>1.5046699999999999E-9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.50149E-9</v>
+      </c>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -1116,16 +1185,19 @@
         <v>8</v>
       </c>
       <c r="E26" s="6">
-        <v>4.1893199999999999E-10</v>
+        <v>4.1069100000000001E-10</v>
       </c>
       <c r="F26" s="6">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G26" s="6">
-        <v>1.46893E-9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.4606900000000001E-9</v>
+      </c>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1139,16 +1211,19 @@
         <v>8</v>
       </c>
       <c r="E27" s="4">
-        <v>6.7306800000000002E-10</v>
+        <v>6.7072100000000005E-10</v>
       </c>
       <c r="F27" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G27" s="4">
-        <v>1.7230699999999999E-9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.72072E-9</v>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1162,16 +1237,19 @@
         <v>8</v>
       </c>
       <c r="E28" s="4">
-        <v>4.8947900000000004E-10</v>
+        <v>4.7161500000000003E-10</v>
       </c>
       <c r="F28" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G28" s="4">
-        <v>1.5394799999999999E-9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.5216100000000001E-9</v>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1185,16 +1263,19 @@
         <v>8</v>
       </c>
       <c r="E29" s="4">
-        <v>4.3581000000000002E-10</v>
+        <v>4.1120300000000001E-10</v>
       </c>
       <c r="F29" s="4">
         <v>1.0500000000000001E-9</v>
       </c>
       <c r="G29" s="4">
-        <v>1.4858100000000001E-9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.4612000000000001E-9</v>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before modifying crit path
</commit_message>
<xml_diff>
--- a/Assignment4/outputs/critical_path_delays.xlsx
+++ b/Assignment4/outputs/critical_path_delays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Acads\Sem7\EE5311_Digital_IC_Design\EE5311-Digital-IC-Design\Assignment4\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0390D0E6-C642-4A3C-9413-7BF457AA0721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1341B600-7896-4E78-A0FA-F717B2CC6BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75A2B2A3-B3E2-432F-A7DC-EC91B0A9FA4A}"/>
   </bookViews>
@@ -64,15 +64,6 @@
     <t>step</t>
   </si>
   <si>
-    <t>crit-path-delay</t>
-  </si>
-  <si>
-    <t>FROM</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -92,6 +83,15 @@
   </si>
   <si>
     <t>Column8</t>
+  </si>
+  <si>
+    <t>Crit-Path-Rise</t>
+  </si>
+  <si>
+    <t>Crit-Path-Fall</t>
+  </si>
+  <si>
+    <t>Max t_pd</t>
   </si>
 </sst>
 </file>
@@ -141,16 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -159,6 +153,14 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,46 +519,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FD03E4-BA0E-4DE5-947F-78562A2D1CD3}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -564,494 +567,601 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
-        <v>3.9237199999999998E-10</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1.4423700000000001E-9</v>
+      <c r="E3" s="6">
+        <v>3.9291900000000002E-10</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3.9665600000000002E-10</v>
+      </c>
+      <c r="G3" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.9665600000000002E-10</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
-        <v>3.5289600000000001E-10</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1.4029E-9</v>
+      <c r="E4" s="6">
+        <v>3.5362799999999998E-10</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3.5374199999999998E-10</v>
+      </c>
+      <c r="G4" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.5374199999999998E-10</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="Q4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4">
-        <v>3.56403E-10</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1.4064E-9</v>
+      <c r="E5" s="6">
+        <v>3.5718800000000002E-10</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3.5467099999999998E-10</v>
+      </c>
+      <c r="G5" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.5718800000000002E-10</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="Q5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4">
-        <v>4.0384000000000002E-10</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1.45384E-9</v>
+      <c r="E6" s="6">
+        <v>4.0449600000000002E-10</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5.3947200000000002E-10</v>
+      </c>
+      <c r="G6" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.3947200000000002E-10</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="4">
-        <v>3.2362100000000002E-10</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1.3736200000000001E-9</v>
+      <c r="E7" s="6">
+        <v>3.2431800000000001E-10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>4.6694800000000001E-10</v>
+      </c>
+      <c r="G7" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>4.6694800000000001E-10</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="4">
-        <v>3.06449E-10</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1.35645E-9</v>
+      <c r="E8" s="6">
+        <v>3.0731900000000002E-10</v>
+      </c>
+      <c r="F8" s="6">
+        <v>4.5805400000000002E-10</v>
+      </c>
+      <c r="G8" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>4.5805400000000002E-10</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4">
-        <v>4.4936499999999998E-10</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1.4993600000000001E-9</v>
+      <c r="E9" s="6">
+        <v>4.4998300000000001E-10</v>
+      </c>
+      <c r="F9" s="6">
+        <v>6.8469499999999998E-10</v>
+      </c>
+      <c r="G9" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>6.8469499999999998E-10</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="4">
-        <v>3.3593700000000001E-10</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1.3859400000000001E-9</v>
+      <c r="E10" s="6">
+        <v>3.3663899999999998E-10</v>
+      </c>
+      <c r="F10" s="6">
+        <v>5.8217500000000001E-10</v>
+      </c>
+      <c r="G10" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.8217500000000001E-10</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="4">
-        <v>3.0555900000000002E-10</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1.35556E-9</v>
+      <c r="E11" s="6">
+        <v>3.06443E-10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5.6370399999999996E-10</v>
+      </c>
+      <c r="G11" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.6370399999999996E-10</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="4">
-        <v>3.8667199999999999E-10</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1.43667E-9</v>
+      <c r="E12" s="6">
+        <v>3.8719300000000001E-10</v>
+      </c>
+      <c r="F12" s="6">
+        <v>3.9047800000000001E-10</v>
+      </c>
+      <c r="G12" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.9047800000000001E-10</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="4">
-        <v>3.4578299999999999E-10</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1.3957799999999999E-9</v>
+      <c r="E13" s="6">
+        <v>3.4652100000000002E-10</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3.46585E-10</v>
+      </c>
+      <c r="G13" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.46585E-10</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="4">
-        <v>3.48026E-10</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1.39803E-9</v>
+      <c r="E14" s="6">
+        <v>3.4882300000000002E-10</v>
+      </c>
+      <c r="F14" s="6">
+        <v>3.4654099999999998E-10</v>
+      </c>
+      <c r="G14" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.4882300000000002E-10</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="4">
-        <v>3.9560199999999997E-10</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1.4456000000000001E-9</v>
+      <c r="E15" s="6">
+        <v>3.96232E-10</v>
+      </c>
+      <c r="F15" s="6">
+        <v>5.3092900000000004E-10</v>
+      </c>
+      <c r="G15" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.3092900000000004E-10</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="4">
-        <v>3.1413599999999998E-10</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1.36414E-9</v>
+      <c r="E16" s="6">
+        <v>3.1491100000000001E-10</v>
+      </c>
+      <c r="F16" s="6">
+        <v>4.57293E-10</v>
+      </c>
+      <c r="G16" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>4.57293E-10</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="4">
-        <v>2.9588600000000002E-10</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1.34589E-9</v>
+      <c r="E17" s="6">
+        <v>2.9667000000000002E-10</v>
+      </c>
+      <c r="F17" s="6">
+        <v>4.4768499999999999E-10</v>
+      </c>
+      <c r="G17" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>4.4768499999999999E-10</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="4">
-        <v>4.39183E-10</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1.48918E-9</v>
+      <c r="E18" s="6">
+        <v>4.39822E-10</v>
+      </c>
+      <c r="F18" s="6">
+        <v>6.7430900000000001E-10</v>
+      </c>
+      <c r="G18" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>6.7430900000000001E-10</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="4">
-        <v>3.2466399999999998E-10</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G19" s="4">
-        <v>1.3746600000000001E-9</v>
+      <c r="E19" s="6">
+        <v>3.2539399999999998E-10</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5.7087000000000001E-10</v>
+      </c>
+      <c r="G19" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.7087000000000001E-10</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="4">
-        <v>2.93227E-10</v>
-      </c>
-      <c r="F20" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1.3432299999999999E-9</v>
+      <c r="E20" s="6">
+        <v>2.9405099999999999E-10</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5.51366E-10</v>
+      </c>
+      <c r="G20" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.51366E-10</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="4">
-        <v>3.8560999999999997E-10</v>
-      </c>
-      <c r="F21" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G21" s="4">
-        <v>1.43561E-9</v>
+      <c r="E21" s="6">
+        <v>3.8617500000000001E-10</v>
+      </c>
+      <c r="F21" s="6">
+        <v>3.8902899999999999E-10</v>
+      </c>
+      <c r="G21" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.8902899999999999E-10</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1064,94 +1174,118 @@
       <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="4">
-        <v>3.4377399999999998E-10</v>
-      </c>
-      <c r="F22" s="4">
-        <v>1.0500000000000001E-9</v>
+      <c r="E22" s="8">
+        <v>3.4451699999999999E-10</v>
+      </c>
+      <c r="F22" s="8">
+        <v>3.4446199999999998E-10</v>
       </c>
       <c r="G22" s="4">
-        <v>1.39377E-9</v>
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.4451699999999999E-10</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="4">
-        <v>3.4519099999999998E-10</v>
-      </c>
-      <c r="F23" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1.39519E-9</v>
+      <c r="E23" s="6">
+        <v>3.4599999999999999E-10</v>
+      </c>
+      <c r="F23" s="6">
+        <v>3.4383300000000002E-10</v>
+      </c>
+      <c r="G23" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>3.4599999999999999E-10</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="4">
-        <v>3.9195500000000002E-10</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1.4419600000000001E-9</v>
+      <c r="E24" s="6">
+        <v>3.9259499999999998E-10</v>
+      </c>
+      <c r="F24" s="6">
+        <v>5.2702699999999996E-10</v>
+      </c>
+      <c r="G24" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.2702699999999996E-10</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="4">
-        <v>3.096E-10</v>
-      </c>
-      <c r="F25" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1.3595999999999999E-9</v>
+      <c r="E25" s="6">
+        <v>3.1037699999999999E-10</v>
+      </c>
+      <c r="F25" s="6">
+        <v>4.52791E-10</v>
+      </c>
+      <c r="G25" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>4.52791E-10</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -1165,94 +1299,130 @@
         <v>8</v>
       </c>
       <c r="E26" s="6">
-        <v>2.8659400000000002E-10</v>
+        <v>2.9152399999999997E-10</v>
       </c>
       <c r="F26" s="6">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G26" s="6">
-        <v>1.34066E-9</v>
+        <v>4.4260800000000002E-10</v>
+      </c>
+      <c r="G26" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>4.4260800000000002E-10</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="4">
-        <v>4.3406300000000002E-10</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G27" s="4">
-        <v>1.4840599999999999E-9</v>
+      <c r="E27" s="6">
+        <v>4.3465900000000002E-10</v>
+      </c>
+      <c r="F27" s="6">
+        <v>6.6913800000000001E-10</v>
+      </c>
+      <c r="G27" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>6.6913800000000001E-10</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="4">
-        <v>3.1869600000000001E-10</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G28" s="4">
-        <v>1.3687E-9</v>
+      <c r="E28" s="6">
+        <v>3.1945500000000001E-10</v>
+      </c>
+      <c r="F28" s="6">
+        <v>5.65047E-10</v>
+      </c>
+      <c r="G28" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.65047E-10</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="4">
-        <v>2.8659400000000002E-10</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1.0500000000000001E-9</v>
-      </c>
-      <c r="G29" s="4">
-        <v>1.33659E-9</v>
+      <c r="E29" s="6">
+        <v>2.8749399999999999E-10</v>
+      </c>
+      <c r="F29" s="6">
+        <v>5.4509799999999999E-10</v>
+      </c>
+      <c r="G29" s="7">
+        <f>MAX(Table2[[#This Row],[Column6]],Table2[[#This Row],[Column7]])</f>
+        <v>5.4509799999999999E-10</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="G31" s="1">
+        <f>MIN(G3:G29)</f>
+        <v>3.4451699999999999E-10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>